<commit_message>
Correct nc emission constraint variants
</commit_message>
<xml_diff>
--- a/SuppXLS/Scen_SYS_ZeroCO2_CAP21-A25E65-nc.xlsx
+++ b/SuppXLS/Scen_SYS_ZeroCO2_CAP21-A25E65-nc.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Olex\Documents\MANRID\ResLab\Modelling\TIMES\TIMES-IE\SuppXLS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CBC99EA1-6BE8-4A08-9669-1B81721D810C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2224DE33-A23B-403E-824A-3E17054F01BC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1900,10 +1900,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{011941A8-04BF-45E8-9F60-D4E07475AB4A}">
-  <dimension ref="A1:S17"/>
+  <dimension ref="A1:AA17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F30" sqref="F30"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="L30" sqref="L30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1911,69 +1911,69 @@
     <col min="1" max="1" width="9.140625" style="8"/>
     <col min="2" max="2" width="14" style="8" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="21.7109375" style="8" bestFit="1" customWidth="1"/>
-    <col min="4" max="5" width="16.42578125" style="8" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="16.42578125" style="8" customWidth="1"/>
-    <col min="7" max="13" width="9.140625" style="8"/>
-    <col min="14" max="14" width="10.5703125" style="8" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="12" style="8" bestFit="1" customWidth="1"/>
-    <col min="16" max="16384" width="9.140625" style="8"/>
+    <col min="4" max="13" width="16.42578125" style="8" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="16.42578125" style="8" customWidth="1"/>
+    <col min="15" max="21" width="9.140625" style="8"/>
+    <col min="22" max="22" width="10.5703125" style="8" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="12" style="8" bestFit="1" customWidth="1"/>
+    <col min="24" max="16384" width="9.140625" style="8"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A1"/>
       <c r="B1"/>
       <c r="C1"/>
-      <c r="E1"/>
-      <c r="G1"/>
-      <c r="H1"/>
-      <c r="I1"/>
-      <c r="J1"/>
-      <c r="K1"/>
-      <c r="L1"/>
       <c r="M1"/>
-      <c r="N1"/>
       <c r="O1"/>
       <c r="P1"/>
       <c r="Q1"/>
       <c r="R1"/>
-    </row>
-    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="S1"/>
+      <c r="T1"/>
+      <c r="U1"/>
+      <c r="V1"/>
+      <c r="W1"/>
+      <c r="X1"/>
+      <c r="Y1"/>
+      <c r="Z1"/>
+    </row>
+    <row r="2" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A2"/>
       <c r="B2"/>
       <c r="C2"/>
-      <c r="E2"/>
-      <c r="G2"/>
-      <c r="H2"/>
-      <c r="I2"/>
-      <c r="J2"/>
-      <c r="K2"/>
-      <c r="L2"/>
       <c r="M2"/>
-      <c r="N2"/>
       <c r="O2"/>
       <c r="P2"/>
       <c r="Q2"/>
       <c r="R2"/>
-    </row>
-    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="S2"/>
+      <c r="T2"/>
+      <c r="U2"/>
+      <c r="V2"/>
+      <c r="W2"/>
+      <c r="X2"/>
+      <c r="Y2"/>
+      <c r="Z2"/>
+    </row>
+    <row r="3" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A3"/>
       <c r="B3"/>
       <c r="C3"/>
-      <c r="E3"/>
-      <c r="G3"/>
-      <c r="H3"/>
-      <c r="I3"/>
-      <c r="J3"/>
-      <c r="K3"/>
-      <c r="L3"/>
       <c r="M3"/>
-      <c r="N3"/>
       <c r="O3"/>
       <c r="P3"/>
       <c r="Q3"/>
       <c r="R3"/>
-    </row>
-    <row r="4" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="S3"/>
+      <c r="T3"/>
+      <c r="U3"/>
+      <c r="V3"/>
+      <c r="W3"/>
+      <c r="X3"/>
+      <c r="Y3"/>
+      <c r="Z3"/>
+    </row>
+    <row r="4" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A4"/>
       <c r="B4" t="s">
         <v>61</v>
@@ -1982,20 +1982,20 @@
         <f xml:space="preserve"> _xlfn.TEXTJOIN("_",TRUE,"UC","NetZero","CO2","2050")</f>
         <v>UC_NetZero_CO2_2050</v>
       </c>
-      <c r="G4"/>
-      <c r="H4"/>
-      <c r="I4"/>
-      <c r="J4"/>
-      <c r="K4"/>
-      <c r="L4"/>
-      <c r="M4"/>
-      <c r="N4"/>
       <c r="O4"/>
       <c r="P4"/>
       <c r="Q4"/>
       <c r="R4"/>
-    </row>
-    <row r="5" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="S4"/>
+      <c r="T4"/>
+      <c r="U4"/>
+      <c r="V4"/>
+      <c r="W4"/>
+      <c r="X4"/>
+      <c r="Y4"/>
+      <c r="Z4"/>
+    </row>
+    <row r="5" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A5"/>
       <c r="B5" t="s">
         <v>66</v>
@@ -2004,20 +2004,20 @@
         <f xml:space="preserve"> _xlfn.TEXTJOIN(" ",TRUE,"Net Zero CO2 by 2050")</f>
         <v>Net Zero CO2 by 2050</v>
       </c>
-      <c r="G5"/>
-      <c r="H5"/>
-      <c r="I5"/>
-      <c r="J5"/>
-      <c r="K5"/>
-      <c r="L5"/>
-      <c r="M5"/>
-      <c r="N5"/>
       <c r="O5"/>
       <c r="P5"/>
       <c r="Q5"/>
       <c r="R5"/>
-    </row>
-    <row r="6" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="S5"/>
+      <c r="T5"/>
+      <c r="U5"/>
+      <c r="V5"/>
+      <c r="W5"/>
+      <c r="X5"/>
+      <c r="Y5"/>
+      <c r="Z5"/>
+    </row>
+    <row r="6" spans="1:27" x14ac:dyDescent="0.25">
       <c r="B6" s="8" t="s">
         <v>72</v>
       </c>
@@ -2028,16 +2028,40 @@
         <v>2021</v>
       </c>
       <c r="E6" s="8">
+        <v>2022</v>
+      </c>
+      <c r="F6" s="8">
+        <v>2023</v>
+      </c>
+      <c r="G6" s="8">
+        <v>2024</v>
+      </c>
+      <c r="H6" s="8">
+        <v>2025</v>
+      </c>
+      <c r="I6" s="8">
+        <v>2026</v>
+      </c>
+      <c r="J6" s="8">
+        <v>2027</v>
+      </c>
+      <c r="K6" s="8">
+        <v>2028</v>
+      </c>
+      <c r="L6" s="8">
+        <v>2029</v>
+      </c>
+      <c r="M6" s="8">
         <v>2030</v>
       </c>
-      <c r="F6" s="8">
+      <c r="N6" s="8">
         <v>2050</v>
       </c>
-      <c r="G6" s="8">
+      <c r="O6" s="8">
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:27" x14ac:dyDescent="0.25">
       <c r="B7" s="8" t="s">
         <v>67</v>
       </c>
@@ -2045,19 +2069,43 @@
         <v>33792</v>
       </c>
       <c r="D7" s="16">
-        <v>35644</v>
+        <v>31606</v>
       </c>
       <c r="E7" s="16">
+        <v>100000</v>
+      </c>
+      <c r="F7" s="16">
+        <v>100000</v>
+      </c>
+      <c r="G7" s="16">
+        <v>100000</v>
+      </c>
+      <c r="H7" s="16">
+        <v>100000</v>
+      </c>
+      <c r="I7" s="16">
+        <v>100000</v>
+      </c>
+      <c r="J7" s="16">
+        <v>100000</v>
+      </c>
+      <c r="K7" s="16">
+        <v>100000</v>
+      </c>
+      <c r="L7" s="16">
+        <v>100000</v>
+      </c>
+      <c r="M7" s="16">
         <v>12482</v>
       </c>
-      <c r="F7" s="16">
+      <c r="N7" s="16">
         <v>0</v>
       </c>
-      <c r="G7" s="8">
+      <c r="O7" s="8">
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:27" x14ac:dyDescent="0.25">
       <c r="B8" s="8" t="s">
         <v>77</v>
       </c>
@@ -2069,15 +2117,47 @@
         <v>T-A*INT*,T-NAV*</v>
       </c>
       <c r="E8" s="8" t="str">
-        <f t="shared" ref="E8:F8" si="0">D8</f>
+        <f t="shared" ref="E8:L8" si="0">D8</f>
         <v>T-A*INT*,T-NAV*</v>
       </c>
       <c r="F8" s="8" t="str">
         <f t="shared" si="0"/>
         <v>T-A*INT*,T-NAV*</v>
       </c>
-    </row>
-    <row r="9" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="G8" s="8" t="str">
+        <f t="shared" si="0"/>
+        <v>T-A*INT*,T-NAV*</v>
+      </c>
+      <c r="H8" s="8" t="str">
+        <f t="shared" si="0"/>
+        <v>T-A*INT*,T-NAV*</v>
+      </c>
+      <c r="I8" s="8" t="str">
+        <f t="shared" si="0"/>
+        <v>T-A*INT*,T-NAV*</v>
+      </c>
+      <c r="J8" s="8" t="str">
+        <f t="shared" si="0"/>
+        <v>T-A*INT*,T-NAV*</v>
+      </c>
+      <c r="K8" s="8" t="str">
+        <f t="shared" si="0"/>
+        <v>T-A*INT*,T-NAV*</v>
+      </c>
+      <c r="L8" s="8" t="str">
+        <f t="shared" si="0"/>
+        <v>T-A*INT*,T-NAV*</v>
+      </c>
+      <c r="M8" s="8" t="str">
+        <f t="shared" ref="M8:N8" si="1">L8</f>
+        <v>T-A*INT*,T-NAV*</v>
+      </c>
+      <c r="N8" s="8" t="str">
+        <f t="shared" si="1"/>
+        <v>T-A*INT*,T-NAV*</v>
+      </c>
+    </row>
+    <row r="9" spans="1:27" x14ac:dyDescent="0.25">
       <c r="B9" s="8" t="s">
         <v>62</v>
       </c>
@@ -2089,15 +2169,47 @@
         <v>*CO2*,-*CO2S</v>
       </c>
       <c r="E9" s="8" t="str">
-        <f t="shared" ref="E9:F9" si="1">D9</f>
+        <f t="shared" ref="E9:L9" si="2">D9</f>
         <v>*CO2*,-*CO2S</v>
       </c>
       <c r="F9" s="8" t="str">
-        <f t="shared" si="1"/>
-        <v>*CO2*,-*CO2S</v>
-      </c>
-    </row>
-    <row r="10" spans="1:19" x14ac:dyDescent="0.25">
+        <f t="shared" si="2"/>
+        <v>*CO2*,-*CO2S</v>
+      </c>
+      <c r="G9" s="8" t="str">
+        <f t="shared" si="2"/>
+        <v>*CO2*,-*CO2S</v>
+      </c>
+      <c r="H9" s="8" t="str">
+        <f t="shared" si="2"/>
+        <v>*CO2*,-*CO2S</v>
+      </c>
+      <c r="I9" s="8" t="str">
+        <f t="shared" si="2"/>
+        <v>*CO2*,-*CO2S</v>
+      </c>
+      <c r="J9" s="8" t="str">
+        <f t="shared" si="2"/>
+        <v>*CO2*,-*CO2S</v>
+      </c>
+      <c r="K9" s="8" t="str">
+        <f t="shared" si="2"/>
+        <v>*CO2*,-*CO2S</v>
+      </c>
+      <c r="L9" s="8" t="str">
+        <f t="shared" si="2"/>
+        <v>*CO2*,-*CO2S</v>
+      </c>
+      <c r="M9" s="8" t="str">
+        <f t="shared" ref="M9:N9" si="3">L9</f>
+        <v>*CO2*,-*CO2S</v>
+      </c>
+      <c r="N9" s="8" t="str">
+        <f t="shared" si="3"/>
+        <v>*CO2*,-*CO2S</v>
+      </c>
+    </row>
+    <row r="10" spans="1:27" x14ac:dyDescent="0.25">
       <c r="B10" s="8" t="s">
         <v>71</v>
       </c>
@@ -2109,20 +2221,52 @@
         <v>ENV</v>
       </c>
       <c r="E10" s="8" t="str">
-        <f t="shared" ref="E10:F10" si="2">D10</f>
+        <f t="shared" ref="E10:L10" si="4">D10</f>
         <v>ENV</v>
       </c>
       <c r="F10" s="8" t="str">
-        <f t="shared" si="2"/>
-        <v>ENV</v>
-      </c>
-    </row>
-    <row r="11" spans="1:19" x14ac:dyDescent="0.25">
+        <f t="shared" si="4"/>
+        <v>ENV</v>
+      </c>
+      <c r="G10" s="8" t="str">
+        <f t="shared" si="4"/>
+        <v>ENV</v>
+      </c>
+      <c r="H10" s="8" t="str">
+        <f t="shared" si="4"/>
+        <v>ENV</v>
+      </c>
+      <c r="I10" s="8" t="str">
+        <f t="shared" si="4"/>
+        <v>ENV</v>
+      </c>
+      <c r="J10" s="8" t="str">
+        <f t="shared" si="4"/>
+        <v>ENV</v>
+      </c>
+      <c r="K10" s="8" t="str">
+        <f t="shared" si="4"/>
+        <v>ENV</v>
+      </c>
+      <c r="L10" s="8" t="str">
+        <f t="shared" si="4"/>
+        <v>ENV</v>
+      </c>
+      <c r="M10" s="8" t="str">
+        <f t="shared" ref="M10:N10" si="5">L10</f>
+        <v>ENV</v>
+      </c>
+      <c r="N10" s="8" t="str">
+        <f t="shared" si="5"/>
+        <v>ENV</v>
+      </c>
+    </row>
+    <row r="11" spans="1:27" x14ac:dyDescent="0.25">
       <c r="B11" s="8" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="12" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:27" x14ac:dyDescent="0.25">
       <c r="B12" s="8" t="s">
         <v>0</v>
       </c>
@@ -2134,15 +2278,47 @@
         <v>UP</v>
       </c>
       <c r="E12" s="8" t="str">
-        <f t="shared" ref="E12:F14" si="3">D12</f>
+        <f t="shared" ref="E12:L12" si="6">D12</f>
         <v>UP</v>
       </c>
       <c r="F12" s="8" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>UP</v>
       </c>
-    </row>
-    <row r="13" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="G12" s="8" t="str">
+        <f t="shared" si="6"/>
+        <v>UP</v>
+      </c>
+      <c r="H12" s="8" t="str">
+        <f t="shared" si="6"/>
+        <v>UP</v>
+      </c>
+      <c r="I12" s="8" t="str">
+        <f t="shared" si="6"/>
+        <v>UP</v>
+      </c>
+      <c r="J12" s="8" t="str">
+        <f t="shared" si="6"/>
+        <v>UP</v>
+      </c>
+      <c r="K12" s="8" t="str">
+        <f t="shared" si="6"/>
+        <v>UP</v>
+      </c>
+      <c r="L12" s="8" t="str">
+        <f t="shared" si="6"/>
+        <v>UP</v>
+      </c>
+      <c r="M12" s="8" t="str">
+        <f t="shared" ref="M12:N12" si="7">L12</f>
+        <v>UP</v>
+      </c>
+      <c r="N12" s="8" t="str">
+        <f t="shared" si="7"/>
+        <v>UP</v>
+      </c>
+    </row>
+    <row r="13" spans="1:27" x14ac:dyDescent="0.25">
       <c r="B13" s="8" t="s">
         <v>79</v>
       </c>
@@ -2150,19 +2326,51 @@
         <v>-1</v>
       </c>
       <c r="D13" s="8">
-        <f t="shared" ref="D13:D14" si="4">C13</f>
+        <f t="shared" ref="D13:L14" si="8">C13</f>
         <v>-1</v>
       </c>
       <c r="E13" s="8">
-        <f t="shared" si="3"/>
+        <f t="shared" si="8"/>
         <v>-1</v>
       </c>
       <c r="F13" s="8">
-        <f t="shared" si="3"/>
+        <f t="shared" si="8"/>
         <v>-1</v>
       </c>
-    </row>
-    <row r="14" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="G13" s="8">
+        <f t="shared" si="8"/>
+        <v>-1</v>
+      </c>
+      <c r="H13" s="8">
+        <f t="shared" si="8"/>
+        <v>-1</v>
+      </c>
+      <c r="I13" s="8">
+        <f t="shared" si="8"/>
+        <v>-1</v>
+      </c>
+      <c r="J13" s="8">
+        <f t="shared" si="8"/>
+        <v>-1</v>
+      </c>
+      <c r="K13" s="8">
+        <f t="shared" si="8"/>
+        <v>-1</v>
+      </c>
+      <c r="L13" s="8">
+        <f t="shared" si="8"/>
+        <v>-1</v>
+      </c>
+      <c r="M13" s="8">
+        <f t="shared" ref="M13:N13" si="9">L13</f>
+        <v>-1</v>
+      </c>
+      <c r="N13" s="8">
+        <f t="shared" si="9"/>
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A14"/>
       <c r="B14" t="s">
         <v>80</v>
@@ -2171,84 +2379,116 @@
         <v>1</v>
       </c>
       <c r="D14" s="8">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>1</v>
       </c>
       <c r="E14" s="8">
-        <f t="shared" si="3"/>
+        <f t="shared" si="8"/>
         <v>1</v>
       </c>
       <c r="F14" s="8">
-        <f t="shared" si="3"/>
+        <f t="shared" si="8"/>
         <v>1</v>
       </c>
-      <c r="G14"/>
-      <c r="H14"/>
-      <c r="I14"/>
-      <c r="J14"/>
-      <c r="K14"/>
-      <c r="L14"/>
-      <c r="M14"/>
-      <c r="N14"/>
+      <c r="G14" s="8">
+        <f t="shared" si="8"/>
+        <v>1</v>
+      </c>
+      <c r="H14" s="8">
+        <f t="shared" si="8"/>
+        <v>1</v>
+      </c>
+      <c r="I14" s="8">
+        <f t="shared" si="8"/>
+        <v>1</v>
+      </c>
+      <c r="J14" s="8">
+        <f t="shared" si="8"/>
+        <v>1</v>
+      </c>
+      <c r="K14" s="8">
+        <f t="shared" si="8"/>
+        <v>1</v>
+      </c>
+      <c r="L14" s="8">
+        <f t="shared" si="8"/>
+        <v>1</v>
+      </c>
+      <c r="M14" s="8">
+        <f t="shared" ref="M14:N14" si="10">L14</f>
+        <v>1</v>
+      </c>
+      <c r="N14" s="8">
+        <f t="shared" si="10"/>
+        <v>1</v>
+      </c>
       <c r="O14"/>
       <c r="P14"/>
       <c r="Q14"/>
       <c r="R14"/>
       <c r="S14"/>
-    </row>
-    <row r="15" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T14"/>
+      <c r="U14"/>
+      <c r="V14"/>
+      <c r="W14"/>
+      <c r="X14"/>
+      <c r="Y14"/>
+      <c r="Z14"/>
+      <c r="AA14"/>
+    </row>
+    <row r="15" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A15"/>
       <c r="B15"/>
       <c r="C15"/>
-      <c r="E15"/>
-      <c r="G15"/>
-      <c r="H15"/>
-      <c r="I15"/>
-      <c r="J15"/>
-      <c r="K15"/>
-      <c r="L15"/>
       <c r="M15"/>
-      <c r="N15"/>
       <c r="O15"/>
       <c r="P15"/>
       <c r="Q15"/>
       <c r="R15"/>
-    </row>
-    <row r="16" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="S15"/>
+      <c r="T15"/>
+      <c r="U15"/>
+      <c r="V15"/>
+      <c r="W15"/>
+      <c r="X15"/>
+      <c r="Y15"/>
+      <c r="Z15"/>
+    </row>
+    <row r="16" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A16"/>
       <c r="B16"/>
       <c r="C16"/>
-      <c r="E16"/>
-      <c r="G16"/>
-      <c r="H16"/>
-      <c r="I16"/>
-      <c r="J16"/>
-      <c r="K16"/>
-      <c r="L16"/>
       <c r="M16"/>
-      <c r="N16"/>
       <c r="O16"/>
       <c r="P16"/>
       <c r="Q16"/>
       <c r="R16"/>
-    </row>
-    <row r="17" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S16"/>
+      <c r="T16"/>
+      <c r="U16"/>
+      <c r="V16"/>
+      <c r="W16"/>
+      <c r="X16"/>
+      <c r="Y16"/>
+      <c r="Z16"/>
+    </row>
+    <row r="17" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A17"/>
       <c r="B17"/>
       <c r="C17"/>
-      <c r="E17"/>
-      <c r="G17"/>
-      <c r="H17"/>
-      <c r="I17"/>
-      <c r="J17"/>
-      <c r="K17"/>
-      <c r="L17"/>
       <c r="M17"/>
-      <c r="N17"/>
       <c r="O17"/>
       <c r="P17"/>
       <c r="Q17"/>
       <c r="R17"/>
+      <c r="S17"/>
+      <c r="T17"/>
+      <c r="U17"/>
+      <c r="V17"/>
+      <c r="W17"/>
+      <c r="X17"/>
+      <c r="Y17"/>
+      <c r="Z17"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2258,10 +2498,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C9318C9B-7F0A-410C-BCB5-F22D93E1F454}">
-  <dimension ref="A1:K15"/>
+  <dimension ref="A1:K31"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E21" sqref="E21"/>
+      <selection activeCell="H31" sqref="H31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2352,48 +2592,48 @@
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B7" s="8" t="str">
-        <f>VLOOKUP(B$5, config!$B$4:$G$14,2,FALSE) &amp; "_Single"</f>
+        <f>VLOOKUP(B$5, config!$B$4:$O$14,2,FALSE) &amp; "_Single"</f>
         <v>UC_NetZero_CO2_2050_Single</v>
       </c>
       <c r="C7" s="8" t="str">
-        <f>VLOOKUP(C$5, config!$B$4:$G$14,MATCH($F7,config!$B$6:$G$6,),FALSE)</f>
+        <f>VLOOKUP(C$5, config!$B$4:$O$14,MATCH($F7,config!$B$6:$O$6,),FALSE)</f>
         <v>*CO2*,-*CO2S</v>
       </c>
       <c r="D7" s="8" t="str">
-        <f>VLOOKUP(D$5, config!$B$4:$G$14,MATCH($F7,config!$B$6:$G$6,),FALSE)</f>
+        <f>VLOOKUP(D$5, config!$B$4:$O$14,MATCH($F7,config!$B$6:$O$6,),FALSE)</f>
         <v>ENV</v>
       </c>
       <c r="F7" s="8">
         <v>2020</v>
       </c>
       <c r="G7" s="8" t="str">
-        <f>VLOOKUP(G$5, config!$B$4:$G$14,MATCH($F7,config!$B$6:$G$6,),FALSE)</f>
+        <f>VLOOKUP(G$5, config!$B$4:$O$14,MATCH($F7,config!$B$6:$O$6,),FALSE)</f>
         <v>UP</v>
       </c>
       <c r="H7" s="8">
-        <f>VLOOKUP(H$5, config!$B$4:$G$14,MATCH($F7,config!$B$6:$G$6,),FALSE)</f>
+        <f>VLOOKUP(H$5, config!$B$4:$O$14,MATCH($F7,config!$B$6:$O$6,),FALSE)</f>
         <v>1</v>
       </c>
       <c r="J7" s="8">
-        <f>VLOOKUP("Value", config!$B$4:$G$14,MATCH($F7,config!$B$6:$G$6,),FALSE)</f>
+        <f>VLOOKUP("Value", config!$B$4:$O$14,MATCH($F7,config!$B$6:$O$6,),FALSE)</f>
         <v>33792</v>
       </c>
       <c r="K7" s="8" t="str">
-        <f>VLOOKUP(K$5, config!$B$4:$G$14,2,FALSE) &amp; " - Single"</f>
+        <f>VLOOKUP(K$5, config!$B$4:$O$14,2,FALSE) &amp; " - Single"</f>
         <v>Net Zero CO2 by 2050 - Single</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="C8" s="8" t="str">
-        <f>VLOOKUP(C$5, config!$B$4:$G$14,MATCH($F8,config!$B$6:$G$6,),FALSE)</f>
+        <f>VLOOKUP(C$5, config!$B$4:$O$14,MATCH($F8,config!$B$6:$O$6,),FALSE)</f>
         <v>*CO2*,-*CO2S</v>
       </c>
       <c r="D8" s="8" t="str">
-        <f>VLOOKUP(D$5, config!$B$4:$G$14,MATCH($F8,config!$B$6:$G$6,),FALSE)</f>
+        <f>VLOOKUP(D$5, config!$B$4:$O$14,MATCH($F8,config!$B$6:$O$6,),FALSE)</f>
         <v>ENV</v>
       </c>
       <c r="E8" s="8" t="str">
-        <f>VLOOKUP(E$5, config!$B$4:$G$14,MATCH($F8,config!$B$6:$G$6,),FALSE)</f>
+        <f>VLOOKUP(E$5, config!$B$4:$O$14,MATCH($F8,config!$B$6:$O$6,),FALSE)</f>
         <v>T-A*INT*,T-NAV*</v>
       </c>
       <c r="F8" s="8">
@@ -2401,46 +2641,46 @@
         <v>2020</v>
       </c>
       <c r="I8" s="8">
-        <f>VLOOKUP(I$5, config!$B$4:$G$14,MATCH($F8,config!$B$6:$G$6,),FALSE)</f>
+        <f>VLOOKUP(I$5, config!$B$4:$O$14,MATCH($F8,config!$B$6:$O$6,),FALSE)</f>
         <v>-1</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="C9" s="8" t="str">
-        <f>VLOOKUP(C$5, config!$B$4:$G$14,MATCH($F9,config!$B$6:$G$6,),FALSE)</f>
+        <f>VLOOKUP(C$5, config!$B$4:$O$14,MATCH($F9,config!$B$6:$O$6,),FALSE)</f>
         <v>*CO2*,-*CO2S</v>
       </c>
       <c r="D9" s="8" t="str">
-        <f>VLOOKUP(D$5, config!$B$4:$G$14,MATCH($F9,config!$B$6:$G$6,),FALSE)</f>
+        <f>VLOOKUP(D$5, config!$B$4:$O$14,MATCH($F9,config!$B$6:$O$6,),FALSE)</f>
         <v>ENV</v>
       </c>
       <c r="F9" s="8">
         <v>2021</v>
       </c>
       <c r="G9" s="8" t="str">
-        <f>VLOOKUP(G$5, config!$B$4:$G$14,MATCH($F9,config!$B$6:$G$6,),FALSE)</f>
+        <f>VLOOKUP(G$5, config!$B$4:$O$14,MATCH($F9,config!$B$6:$O$6,),FALSE)</f>
         <v>UP</v>
       </c>
       <c r="H9" s="8">
-        <f>VLOOKUP(H$5, config!$B$4:$G$14,MATCH($F9,config!$B$6:$G$6,),FALSE)</f>
+        <f>VLOOKUP(H$5, config!$B$4:$O$14,MATCH($F9,config!$B$6:$O$6,),FALSE)</f>
         <v>1</v>
       </c>
       <c r="J9" s="8">
-        <f>VLOOKUP("Value", config!$B$4:$G$14,MATCH($F9,config!$B$6:$G$6,),FALSE)</f>
-        <v>35644</v>
+        <f>VLOOKUP("Value", config!$B$4:$O$14,MATCH($F9,config!$B$6:$O$6,),FALSE)</f>
+        <v>31606</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="C10" s="8" t="str">
-        <f>VLOOKUP(C$5, config!$B$4:$G$14,MATCH($F10,config!$B$6:$G$6,),FALSE)</f>
+        <f>VLOOKUP(C$5, config!$B$4:$O$14,MATCH($F10,config!$B$6:$O$6,),FALSE)</f>
         <v>*CO2*,-*CO2S</v>
       </c>
       <c r="D10" s="8" t="str">
-        <f>VLOOKUP(D$5, config!$B$4:$G$14,MATCH($F10,config!$B$6:$G$6,),FALSE)</f>
+        <f>VLOOKUP(D$5, config!$B$4:$O$14,MATCH($F10,config!$B$6:$O$6,),FALSE)</f>
         <v>ENV</v>
       </c>
       <c r="E10" s="8" t="str">
-        <f>VLOOKUP(E$5, config!$B$4:$G$14,MATCH($F10,config!$B$6:$G$6,),FALSE)</f>
+        <f>VLOOKUP(E$5, config!$B$4:$O$14,MATCH($F10,config!$B$6:$O$6,),FALSE)</f>
         <v>T-A*INT*,T-NAV*</v>
       </c>
       <c r="F10" s="8">
@@ -2448,110 +2688,486 @@
         <v>2021</v>
       </c>
       <c r="I10" s="8">
-        <f>VLOOKUP(I$5, config!$B$4:$G$14,MATCH($F10,config!$B$6:$G$6,),FALSE)</f>
+        <f>VLOOKUP(I$5, config!$B$4:$O$14,MATCH($F10,config!$B$6:$O$6,),FALSE)</f>
         <v>-1</v>
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="C11" s="8" t="str">
-        <f>VLOOKUP(C$5, config!$B$4:$G$14,MATCH($F11,config!$B$6:$G$6,),FALSE)</f>
+        <f>VLOOKUP(C$5, config!$B$4:$O$14,MATCH($F11,config!$B$6:$O$6,),FALSE)</f>
         <v>*CO2*,-*CO2S</v>
       </c>
       <c r="D11" s="8" t="str">
-        <f>VLOOKUP(D$5, config!$B$4:$G$14,MATCH($F11,config!$B$6:$G$6,),FALSE)</f>
+        <f>VLOOKUP(D$5, config!$B$4:$O$14,MATCH($F11,config!$B$6:$O$6,),FALSE)</f>
         <v>ENV</v>
       </c>
       <c r="F11" s="8">
-        <v>2030</v>
+        <v>2022</v>
       </c>
       <c r="G11" s="8" t="str">
-        <f>VLOOKUP(G$5, config!$B$4:$G$14,MATCH($F11,config!$B$6:$G$6,),FALSE)</f>
+        <f>VLOOKUP(G$5, config!$B$4:$O$14,MATCH($F11,config!$B$6:$O$6,),FALSE)</f>
         <v>UP</v>
       </c>
       <c r="H11" s="8">
-        <f>VLOOKUP(H$5, config!$B$4:$G$14,MATCH($F11,config!$B$6:$G$6,),FALSE)</f>
+        <f>VLOOKUP(H$5, config!$B$4:$O$14,MATCH($F11,config!$B$6:$O$6,),FALSE)</f>
         <v>1</v>
       </c>
       <c r="J11" s="8">
-        <f>VLOOKUP("Value", config!$B$4:$G$14,MATCH($F11,config!$B$6:$G$6,),FALSE)</f>
-        <v>12482</v>
+        <f>VLOOKUP("Value", config!$B$4:$O$14,MATCH($F11,config!$B$6:$O$6,),FALSE)</f>
+        <v>100000</v>
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="C12" s="8" t="str">
-        <f>VLOOKUP(C$5, config!$B$4:$G$14,MATCH($F12,config!$B$6:$G$6,),FALSE)</f>
+        <f>VLOOKUP(C$5, config!$B$4:$O$14,MATCH($F12,config!$B$6:$O$6,),FALSE)</f>
         <v>*CO2*,-*CO2S</v>
       </c>
       <c r="D12" s="8" t="str">
-        <f>VLOOKUP(D$5, config!$B$4:$G$14,MATCH($F12,config!$B$6:$G$6,),FALSE)</f>
+        <f>VLOOKUP(D$5, config!$B$4:$O$14,MATCH($F12,config!$B$6:$O$6,),FALSE)</f>
         <v>ENV</v>
       </c>
       <c r="E12" s="8" t="str">
-        <f>VLOOKUP(E$5, config!$B$4:$G$14,MATCH($F12,config!$B$6:$G$6,),FALSE)</f>
+        <f>VLOOKUP(E$5, config!$B$4:$O$14,MATCH($F12,config!$B$6:$O$6,),FALSE)</f>
         <v>T-A*INT*,T-NAV*</v>
       </c>
       <c r="F12" s="8">
         <f>F11</f>
-        <v>2030</v>
+        <v>2022</v>
       </c>
       <c r="I12" s="8">
-        <f>VLOOKUP(I$5, config!$B$4:$G$14,MATCH($F12,config!$B$6:$G$6,),FALSE)</f>
+        <f>VLOOKUP(I$5, config!$B$4:$O$14,MATCH($F12,config!$B$6:$O$6,),FALSE)</f>
         <v>-1</v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="C13" s="8" t="str">
-        <f>VLOOKUP(C$5, config!$B$4:$G$14,MATCH($F13,config!$B$6:$G$6,),FALSE)</f>
+        <f>VLOOKUP(C$5, config!$B$4:$O$14,MATCH($F13,config!$B$6:$O$6,),FALSE)</f>
         <v>*CO2*,-*CO2S</v>
       </c>
       <c r="D13" s="8" t="str">
-        <f>VLOOKUP(D$5, config!$B$4:$G$14,MATCH($F13,config!$B$6:$G$6,),FALSE)</f>
+        <f>VLOOKUP(D$5, config!$B$4:$O$14,MATCH($F13,config!$B$6:$O$6,),FALSE)</f>
         <v>ENV</v>
       </c>
       <c r="F13" s="8">
-        <v>2050</v>
+        <v>2023</v>
       </c>
       <c r="G13" s="8" t="str">
-        <f>VLOOKUP(G$5, config!$B$4:$G$14,MATCH($F13,config!$B$6:$G$6,),FALSE)</f>
+        <f>VLOOKUP(G$5, config!$B$4:$O$14,MATCH($F13,config!$B$6:$O$6,),FALSE)</f>
         <v>UP</v>
       </c>
       <c r="H13" s="8">
-        <f>VLOOKUP(H$5, config!$B$4:$G$14,MATCH($F13,config!$B$6:$G$6,),FALSE)</f>
+        <f>VLOOKUP(H$5, config!$B$4:$O$14,MATCH($F13,config!$B$6:$O$6,),FALSE)</f>
         <v>1</v>
       </c>
       <c r="J13" s="8">
-        <f>VLOOKUP("Value", config!$B$4:$G$14,MATCH($F13,config!$B$6:$G$6,),FALSE)</f>
-        <v>0</v>
+        <f>VLOOKUP("Value", config!$B$4:$O$14,MATCH($F13,config!$B$6:$O$6,),FALSE)</f>
+        <v>100000</v>
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="C14" s="8" t="str">
-        <f>VLOOKUP(C$5, config!$B$4:$G$14,MATCH($F14,config!$B$6:$G$6,),FALSE)</f>
+        <f>VLOOKUP(C$5, config!$B$4:$O$14,MATCH($F14,config!$B$6:$O$6,),FALSE)</f>
         <v>*CO2*,-*CO2S</v>
       </c>
       <c r="D14" s="8" t="str">
-        <f>VLOOKUP(D$5, config!$B$4:$G$14,MATCH($F14,config!$B$6:$G$6,),FALSE)</f>
+        <f>VLOOKUP(D$5, config!$B$4:$O$14,MATCH($F14,config!$B$6:$O$6,),FALSE)</f>
         <v>ENV</v>
       </c>
       <c r="E14" s="8" t="str">
-        <f>VLOOKUP(E$5, config!$B$4:$G$14,MATCH($F14,config!$B$6:$G$6,),FALSE)</f>
+        <f>VLOOKUP(E$5, config!$B$4:$O$14,MATCH($F14,config!$B$6:$O$6,),FALSE)</f>
         <v>T-A*INT*,T-NAV*</v>
       </c>
       <c r="F14" s="8">
         <f>F13</f>
+        <v>2023</v>
+      </c>
+      <c r="I14" s="8">
+        <f>VLOOKUP(I$5, config!$B$4:$O$14,MATCH($F14,config!$B$6:$O$6,),FALSE)</f>
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="C15" s="8" t="str">
+        <f>VLOOKUP(C$5, config!$B$4:$O$14,MATCH($F15,config!$B$6:$O$6,),FALSE)</f>
+        <v>*CO2*,-*CO2S</v>
+      </c>
+      <c r="D15" s="8" t="str">
+        <f>VLOOKUP(D$5, config!$B$4:$O$14,MATCH($F15,config!$B$6:$O$6,),FALSE)</f>
+        <v>ENV</v>
+      </c>
+      <c r="F15" s="8">
+        <v>2024</v>
+      </c>
+      <c r="G15" s="8" t="str">
+        <f>VLOOKUP(G$5, config!$B$4:$O$14,MATCH($F15,config!$B$6:$O$6,),FALSE)</f>
+        <v>UP</v>
+      </c>
+      <c r="H15" s="8">
+        <f>VLOOKUP(H$5, config!$B$4:$O$14,MATCH($F15,config!$B$6:$O$6,),FALSE)</f>
+        <v>1</v>
+      </c>
+      <c r="J15" s="8">
+        <f>VLOOKUP("Value", config!$B$4:$O$14,MATCH($F15,config!$B$6:$O$6,),FALSE)</f>
+        <v>100000</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="C16" s="8" t="str">
+        <f>VLOOKUP(C$5, config!$B$4:$O$14,MATCH($F16,config!$B$6:$O$6,),FALSE)</f>
+        <v>*CO2*,-*CO2S</v>
+      </c>
+      <c r="D16" s="8" t="str">
+        <f>VLOOKUP(D$5, config!$B$4:$O$14,MATCH($F16,config!$B$6:$O$6,),FALSE)</f>
+        <v>ENV</v>
+      </c>
+      <c r="E16" s="8" t="str">
+        <f>VLOOKUP(E$5, config!$B$4:$O$14,MATCH($F16,config!$B$6:$O$6,),FALSE)</f>
+        <v>T-A*INT*,T-NAV*</v>
+      </c>
+      <c r="F16" s="8">
+        <f>F15</f>
+        <v>2024</v>
+      </c>
+      <c r="I16" s="8">
+        <f>VLOOKUP(I$5, config!$B$4:$O$14,MATCH($F16,config!$B$6:$O$6,),FALSE)</f>
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="17" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C17" s="8" t="str">
+        <f>VLOOKUP(C$5, config!$B$4:$O$14,MATCH($F17,config!$B$6:$O$6,),FALSE)</f>
+        <v>*CO2*,-*CO2S</v>
+      </c>
+      <c r="D17" s="8" t="str">
+        <f>VLOOKUP(D$5, config!$B$4:$O$14,MATCH($F17,config!$B$6:$O$6,),FALSE)</f>
+        <v>ENV</v>
+      </c>
+      <c r="F17" s="8">
+        <v>2025</v>
+      </c>
+      <c r="G17" s="8" t="str">
+        <f>VLOOKUP(G$5, config!$B$4:$O$14,MATCH($F17,config!$B$6:$O$6,),FALSE)</f>
+        <v>UP</v>
+      </c>
+      <c r="H17" s="8">
+        <f>VLOOKUP(H$5, config!$B$4:$O$14,MATCH($F17,config!$B$6:$O$6,),FALSE)</f>
+        <v>1</v>
+      </c>
+      <c r="J17" s="8">
+        <f>VLOOKUP("Value", config!$B$4:$O$14,MATCH($F17,config!$B$6:$O$6,),FALSE)</f>
+        <v>100000</v>
+      </c>
+    </row>
+    <row r="18" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C18" s="8" t="str">
+        <f>VLOOKUP(C$5, config!$B$4:$O$14,MATCH($F18,config!$B$6:$O$6,),FALSE)</f>
+        <v>*CO2*,-*CO2S</v>
+      </c>
+      <c r="D18" s="8" t="str">
+        <f>VLOOKUP(D$5, config!$B$4:$O$14,MATCH($F18,config!$B$6:$O$6,),FALSE)</f>
+        <v>ENV</v>
+      </c>
+      <c r="E18" s="8" t="str">
+        <f>VLOOKUP(E$5, config!$B$4:$O$14,MATCH($F18,config!$B$6:$O$6,),FALSE)</f>
+        <v>T-A*INT*,T-NAV*</v>
+      </c>
+      <c r="F18" s="8">
+        <f>F17</f>
+        <v>2025</v>
+      </c>
+      <c r="I18" s="8">
+        <f>VLOOKUP(I$5, config!$B$4:$O$14,MATCH($F18,config!$B$6:$O$6,),FALSE)</f>
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="19" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C19" s="8" t="str">
+        <f>VLOOKUP(C$5, config!$B$4:$O$14,MATCH($F19,config!$B$6:$O$6,),FALSE)</f>
+        <v>*CO2*,-*CO2S</v>
+      </c>
+      <c r="D19" s="8" t="str">
+        <f>VLOOKUP(D$5, config!$B$4:$O$14,MATCH($F19,config!$B$6:$O$6,),FALSE)</f>
+        <v>ENV</v>
+      </c>
+      <c r="F19" s="8">
+        <v>2026</v>
+      </c>
+      <c r="G19" s="8" t="str">
+        <f>VLOOKUP(G$5, config!$B$4:$O$14,MATCH($F19,config!$B$6:$O$6,),FALSE)</f>
+        <v>UP</v>
+      </c>
+      <c r="H19" s="8">
+        <f>VLOOKUP(H$5, config!$B$4:$O$14,MATCH($F19,config!$B$6:$O$6,),FALSE)</f>
+        <v>1</v>
+      </c>
+      <c r="J19" s="8">
+        <f>VLOOKUP("Value", config!$B$4:$O$14,MATCH($F19,config!$B$6:$O$6,),FALSE)</f>
+        <v>100000</v>
+      </c>
+    </row>
+    <row r="20" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C20" s="8" t="str">
+        <f>VLOOKUP(C$5, config!$B$4:$O$14,MATCH($F20,config!$B$6:$O$6,),FALSE)</f>
+        <v>*CO2*,-*CO2S</v>
+      </c>
+      <c r="D20" s="8" t="str">
+        <f>VLOOKUP(D$5, config!$B$4:$O$14,MATCH($F20,config!$B$6:$O$6,),FALSE)</f>
+        <v>ENV</v>
+      </c>
+      <c r="E20" s="8" t="str">
+        <f>VLOOKUP(E$5, config!$B$4:$O$14,MATCH($F20,config!$B$6:$O$6,),FALSE)</f>
+        <v>T-A*INT*,T-NAV*</v>
+      </c>
+      <c r="F20" s="8">
+        <f>F19</f>
+        <v>2026</v>
+      </c>
+      <c r="I20" s="8">
+        <f>VLOOKUP(I$5, config!$B$4:$O$14,MATCH($F20,config!$B$6:$O$6,),FALSE)</f>
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="21" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C21" s="8" t="str">
+        <f>VLOOKUP(C$5, config!$B$4:$O$14,MATCH($F21,config!$B$6:$O$6,),FALSE)</f>
+        <v>*CO2*,-*CO2S</v>
+      </c>
+      <c r="D21" s="8" t="str">
+        <f>VLOOKUP(D$5, config!$B$4:$O$14,MATCH($F21,config!$B$6:$O$6,),FALSE)</f>
+        <v>ENV</v>
+      </c>
+      <c r="F21" s="8">
+        <v>2027</v>
+      </c>
+      <c r="G21" s="8" t="str">
+        <f>VLOOKUP(G$5, config!$B$4:$O$14,MATCH($F21,config!$B$6:$O$6,),FALSE)</f>
+        <v>UP</v>
+      </c>
+      <c r="H21" s="8">
+        <f>VLOOKUP(H$5, config!$B$4:$O$14,MATCH($F21,config!$B$6:$O$6,),FALSE)</f>
+        <v>1</v>
+      </c>
+      <c r="J21" s="8">
+        <f>VLOOKUP("Value", config!$B$4:$O$14,MATCH($F21,config!$B$6:$O$6,),FALSE)</f>
+        <v>100000</v>
+      </c>
+    </row>
+    <row r="22" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C22" s="8" t="str">
+        <f>VLOOKUP(C$5, config!$B$4:$O$14,MATCH($F22,config!$B$6:$O$6,),FALSE)</f>
+        <v>*CO2*,-*CO2S</v>
+      </c>
+      <c r="D22" s="8" t="str">
+        <f>VLOOKUP(D$5, config!$B$4:$O$14,MATCH($F22,config!$B$6:$O$6,),FALSE)</f>
+        <v>ENV</v>
+      </c>
+      <c r="E22" s="8" t="str">
+        <f>VLOOKUP(E$5, config!$B$4:$O$14,MATCH($F22,config!$B$6:$O$6,),FALSE)</f>
+        <v>T-A*INT*,T-NAV*</v>
+      </c>
+      <c r="F22" s="8">
+        <f>F21</f>
+        <v>2027</v>
+      </c>
+      <c r="I22" s="8">
+        <f>VLOOKUP(I$5, config!$B$4:$O$14,MATCH($F22,config!$B$6:$O$6,),FALSE)</f>
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="23" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C23" s="8" t="str">
+        <f>VLOOKUP(C$5, config!$B$4:$O$14,MATCH($F23,config!$B$6:$O$6,),FALSE)</f>
+        <v>*CO2*,-*CO2S</v>
+      </c>
+      <c r="D23" s="8" t="str">
+        <f>VLOOKUP(D$5, config!$B$4:$O$14,MATCH($F23,config!$B$6:$O$6,),FALSE)</f>
+        <v>ENV</v>
+      </c>
+      <c r="F23" s="8">
+        <v>2028</v>
+      </c>
+      <c r="G23" s="8" t="str">
+        <f>VLOOKUP(G$5, config!$B$4:$O$14,MATCH($F23,config!$B$6:$O$6,),FALSE)</f>
+        <v>UP</v>
+      </c>
+      <c r="H23" s="8">
+        <f>VLOOKUP(H$5, config!$B$4:$O$14,MATCH($F23,config!$B$6:$O$6,),FALSE)</f>
+        <v>1</v>
+      </c>
+      <c r="J23" s="8">
+        <f>VLOOKUP("Value", config!$B$4:$O$14,MATCH($F23,config!$B$6:$O$6,),FALSE)</f>
+        <v>100000</v>
+      </c>
+    </row>
+    <row r="24" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C24" s="8" t="str">
+        <f>VLOOKUP(C$5, config!$B$4:$O$14,MATCH($F24,config!$B$6:$O$6,),FALSE)</f>
+        <v>*CO2*,-*CO2S</v>
+      </c>
+      <c r="D24" s="8" t="str">
+        <f>VLOOKUP(D$5, config!$B$4:$O$14,MATCH($F24,config!$B$6:$O$6,),FALSE)</f>
+        <v>ENV</v>
+      </c>
+      <c r="E24" s="8" t="str">
+        <f>VLOOKUP(E$5, config!$B$4:$O$14,MATCH($F24,config!$B$6:$O$6,),FALSE)</f>
+        <v>T-A*INT*,T-NAV*</v>
+      </c>
+      <c r="F24" s="8">
+        <f>F23</f>
+        <v>2028</v>
+      </c>
+      <c r="I24" s="8">
+        <f>VLOOKUP(I$5, config!$B$4:$O$14,MATCH($F24,config!$B$6:$O$6,),FALSE)</f>
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="25" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C25" s="8" t="str">
+        <f>VLOOKUP(C$5, config!$B$4:$O$14,MATCH($F25,config!$B$6:$O$6,),FALSE)</f>
+        <v>*CO2*,-*CO2S</v>
+      </c>
+      <c r="D25" s="8" t="str">
+        <f>VLOOKUP(D$5, config!$B$4:$O$14,MATCH($F25,config!$B$6:$O$6,),FALSE)</f>
+        <v>ENV</v>
+      </c>
+      <c r="F25" s="8">
+        <v>2029</v>
+      </c>
+      <c r="G25" s="8" t="str">
+        <f>VLOOKUP(G$5, config!$B$4:$O$14,MATCH($F25,config!$B$6:$O$6,),FALSE)</f>
+        <v>UP</v>
+      </c>
+      <c r="H25" s="8">
+        <f>VLOOKUP(H$5, config!$B$4:$O$14,MATCH($F25,config!$B$6:$O$6,),FALSE)</f>
+        <v>1</v>
+      </c>
+      <c r="J25" s="8">
+        <f>VLOOKUP("Value", config!$B$4:$O$14,MATCH($F25,config!$B$6:$O$6,),FALSE)</f>
+        <v>100000</v>
+      </c>
+    </row>
+    <row r="26" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C26" s="8" t="str">
+        <f>VLOOKUP(C$5, config!$B$4:$O$14,MATCH($F26,config!$B$6:$O$6,),FALSE)</f>
+        <v>*CO2*,-*CO2S</v>
+      </c>
+      <c r="D26" s="8" t="str">
+        <f>VLOOKUP(D$5, config!$B$4:$O$14,MATCH($F26,config!$B$6:$O$6,),FALSE)</f>
+        <v>ENV</v>
+      </c>
+      <c r="E26" s="8" t="str">
+        <f>VLOOKUP(E$5, config!$B$4:$O$14,MATCH($F26,config!$B$6:$O$6,),FALSE)</f>
+        <v>T-A*INT*,T-NAV*</v>
+      </c>
+      <c r="F26" s="8">
+        <f>F25</f>
+        <v>2029</v>
+      </c>
+      <c r="I26" s="8">
+        <f>VLOOKUP(I$5, config!$B$4:$O$14,MATCH($F26,config!$B$6:$O$6,),FALSE)</f>
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="27" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C27" s="8" t="str">
+        <f>VLOOKUP(C$5, config!$B$4:$O$14,MATCH($F27,config!$B$6:$O$6,),FALSE)</f>
+        <v>*CO2*,-*CO2S</v>
+      </c>
+      <c r="D27" s="8" t="str">
+        <f>VLOOKUP(D$5, config!$B$4:$O$14,MATCH($F27,config!$B$6:$O$6,),FALSE)</f>
+        <v>ENV</v>
+      </c>
+      <c r="F27" s="8">
+        <v>2030</v>
+      </c>
+      <c r="G27" s="8" t="str">
+        <f>VLOOKUP(G$5, config!$B$4:$O$14,MATCH($F27,config!$B$6:$O$6,),FALSE)</f>
+        <v>UP</v>
+      </c>
+      <c r="H27" s="8">
+        <f>VLOOKUP(H$5, config!$B$4:$O$14,MATCH($F27,config!$B$6:$O$6,),FALSE)</f>
+        <v>1</v>
+      </c>
+      <c r="J27" s="8">
+        <f>VLOOKUP("Value", config!$B$4:$O$14,MATCH($F27,config!$B$6:$O$6,),FALSE)</f>
+        <v>12482</v>
+      </c>
+    </row>
+    <row r="28" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C28" s="8" t="str">
+        <f>VLOOKUP(C$5, config!$B$4:$O$14,MATCH($F28,config!$B$6:$O$6,),FALSE)</f>
+        <v>*CO2*,-*CO2S</v>
+      </c>
+      <c r="D28" s="8" t="str">
+        <f>VLOOKUP(D$5, config!$B$4:$O$14,MATCH($F28,config!$B$6:$O$6,),FALSE)</f>
+        <v>ENV</v>
+      </c>
+      <c r="E28" s="8" t="str">
+        <f>VLOOKUP(E$5, config!$B$4:$O$14,MATCH($F28,config!$B$6:$O$6,),FALSE)</f>
+        <v>T-A*INT*,T-NAV*</v>
+      </c>
+      <c r="F28" s="8">
+        <f>F27</f>
+        <v>2030</v>
+      </c>
+      <c r="I28" s="8">
+        <f>VLOOKUP(I$5, config!$B$4:$O$14,MATCH($F28,config!$B$6:$O$6,),FALSE)</f>
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="29" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C29" s="8" t="str">
+        <f>VLOOKUP(C$5, config!$B$4:$O$14,MATCH($F29,config!$B$6:$O$6,),FALSE)</f>
+        <v>*CO2*,-*CO2S</v>
+      </c>
+      <c r="D29" s="8" t="str">
+        <f>VLOOKUP(D$5, config!$B$4:$O$14,MATCH($F29,config!$B$6:$O$6,),FALSE)</f>
+        <v>ENV</v>
+      </c>
+      <c r="F29" s="8">
         <v>2050</v>
       </c>
-      <c r="I14" s="8">
-        <f>VLOOKUP(I$5, config!$B$4:$G$14,MATCH($F14,config!$B$6:$G$6,),FALSE)</f>
+      <c r="G29" s="8" t="str">
+        <f>VLOOKUP(G$5, config!$B$4:$O$14,MATCH($F29,config!$B$6:$O$6,),FALSE)</f>
+        <v>UP</v>
+      </c>
+      <c r="H29" s="8">
+        <f>VLOOKUP(H$5, config!$B$4:$O$14,MATCH($F29,config!$B$6:$O$6,),FALSE)</f>
+        <v>1</v>
+      </c>
+      <c r="J29" s="8">
+        <f>VLOOKUP("Value", config!$B$4:$O$14,MATCH($F29,config!$B$6:$O$6,),FALSE)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C30" s="8" t="str">
+        <f>VLOOKUP(C$5, config!$B$4:$O$14,MATCH($F30,config!$B$6:$O$6,),FALSE)</f>
+        <v>*CO2*,-*CO2S</v>
+      </c>
+      <c r="D30" s="8" t="str">
+        <f>VLOOKUP(D$5, config!$B$4:$O$14,MATCH($F30,config!$B$6:$O$6,),FALSE)</f>
+        <v>ENV</v>
+      </c>
+      <c r="E30" s="8" t="str">
+        <f>VLOOKUP(E$5, config!$B$4:$O$14,MATCH($F30,config!$B$6:$O$6,),FALSE)</f>
+        <v>T-A*INT*,T-NAV*</v>
+      </c>
+      <c r="F30" s="8">
+        <f>F29</f>
+        <v>2050</v>
+      </c>
+      <c r="I30" s="8">
+        <f>VLOOKUP(I$5, config!$B$4:$O$14,MATCH($F30,config!$B$6:$O$6,),FALSE)</f>
         <v>-1</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="F15" s="8">
+    <row r="31" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="F31" s="8">
         <v>0</v>
       </c>
-      <c r="J15" s="8">
-        <f>VLOOKUP("Value", config!$B$4:$G$14,MATCH($F15,config!$B$6:$G$6,),FALSE)</f>
+      <c r="J31" s="8">
+        <f>VLOOKUP("Value", config!$B$4:$O$14,MATCH($F31,config!$B$6:$O$6,),FALSE)</f>
         <v>5</v>
       </c>
     </row>
@@ -2563,10 +3179,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E6EC2971-91FC-4261-B0BB-58C7F43C1746}">
-  <dimension ref="A1:K15"/>
+  <dimension ref="A1:K31"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="K29" sqref="K29"/>
+      <selection activeCell="A29" sqref="A29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2657,48 +3273,48 @@
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B7" s="8" t="str">
-        <f>VLOOKUP(B$5, config!$B$4:$G$14,2,FALSE) &amp; "_Multi"</f>
+        <f>VLOOKUP(B$5, config!$B$4:$O$14,2,FALSE) &amp; "_Multi"</f>
         <v>UC_NetZero_CO2_2050_Multi</v>
       </c>
       <c r="C7" s="8" t="str">
-        <f>VLOOKUP(C$5, config!$B$4:$G$14,MATCH($F7,config!$B$6:$G$6,),FALSE)</f>
+        <f>VLOOKUP(C$5, config!$B$4:$O$14,MATCH($F7,config!$B$6:$O$6,),FALSE)</f>
         <v>*CO2*,-*CO2S</v>
       </c>
       <c r="D7" s="8" t="str">
-        <f>VLOOKUP(D$5, config!$B$4:$G$14,MATCH($F7,config!$B$6:$G$6,),FALSE)</f>
+        <f>VLOOKUP(D$5, config!$B$4:$O$14,MATCH($F7,config!$B$6:$O$6,),FALSE)</f>
         <v>ENV</v>
       </c>
       <c r="F7" s="8">
         <v>2020</v>
       </c>
       <c r="G7" s="8" t="str">
-        <f>VLOOKUP(G$5, config!$B$4:$G$14,MATCH($F7,config!$B$6:$G$6,),FALSE)</f>
+        <f>VLOOKUP(G$5, config!$B$4:$O$14,MATCH($F7,config!$B$6:$O$6,),FALSE)</f>
         <v>UP</v>
       </c>
       <c r="H7" s="8">
-        <f>VLOOKUP(H$5, config!$B$4:$G$14,MATCH($F7,config!$B$6:$G$6,),FALSE)</f>
+        <f>VLOOKUP(H$5, config!$B$4:$O$14,MATCH($F7,config!$B$6:$O$6,),FALSE)</f>
         <v>1</v>
       </c>
       <c r="J7" s="8">
-        <f>VLOOKUP("Value", config!$B$4:$G$14,MATCH($F7,config!$B$6:$G$6,),FALSE)</f>
+        <f>VLOOKUP("Value", config!$B$4:$O$14,MATCH($F7,config!$B$6:$O$6,),FALSE)</f>
         <v>33792</v>
       </c>
       <c r="K7" s="8" t="str">
-        <f>VLOOKUP(K$5, config!$B$4:$G$14,2,FALSE) &amp; " - Multi"</f>
+        <f>VLOOKUP(K$5, config!$B$4:$O$14,2,FALSE) &amp; " - Multi"</f>
         <v>Net Zero CO2 by 2050 - Multi</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="C8" s="8" t="str">
-        <f>VLOOKUP(C$5, config!$B$4:$G$14,MATCH($F8,config!$B$6:$G$6,),FALSE)</f>
+        <f>VLOOKUP(C$5, config!$B$4:$O$14,MATCH($F8,config!$B$6:$O$6,),FALSE)</f>
         <v>*CO2*,-*CO2S</v>
       </c>
       <c r="D8" s="8" t="str">
-        <f>VLOOKUP(D$5, config!$B$4:$G$14,MATCH($F8,config!$B$6:$G$6,),FALSE)</f>
+        <f>VLOOKUP(D$5, config!$B$4:$O$14,MATCH($F8,config!$B$6:$O$6,),FALSE)</f>
         <v>ENV</v>
       </c>
       <c r="E8" s="8" t="str">
-        <f>VLOOKUP(E$5, config!$B$4:$G$14,MATCH($F8,config!$B$6:$G$6,),FALSE)</f>
+        <f>VLOOKUP(E$5, config!$B$4:$O$14,MATCH($F8,config!$B$6:$O$6,),FALSE)</f>
         <v>T-A*INT*,T-NAV*</v>
       </c>
       <c r="F8" s="8">
@@ -2706,46 +3322,46 @@
         <v>2020</v>
       </c>
       <c r="I8" s="8">
-        <f>VLOOKUP(I$5, config!$B$4:$G$14,MATCH($F8,config!$B$6:$G$6,),FALSE)</f>
+        <f>VLOOKUP(I$5, config!$B$4:$O$14,MATCH($F8,config!$B$6:$O$6,),FALSE)</f>
         <v>-1</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="C9" s="8" t="str">
-        <f>VLOOKUP(C$5, config!$B$4:$G$14,MATCH($F9,config!$B$6:$G$6,),FALSE)</f>
+        <f>VLOOKUP(C$5, config!$B$4:$O$14,MATCH($F9,config!$B$6:$O$6,),FALSE)</f>
         <v>*CO2*,-*CO2S</v>
       </c>
       <c r="D9" s="8" t="str">
-        <f>VLOOKUP(D$5, config!$B$4:$G$14,MATCH($F9,config!$B$6:$G$6,),FALSE)</f>
+        <f>VLOOKUP(D$5, config!$B$4:$O$14,MATCH($F9,config!$B$6:$O$6,),FALSE)</f>
         <v>ENV</v>
       </c>
       <c r="F9" s="8">
         <v>2021</v>
       </c>
       <c r="G9" s="8" t="str">
-        <f>VLOOKUP(G$5, config!$B$4:$G$14,MATCH($F9,config!$B$6:$G$6,),FALSE)</f>
+        <f>VLOOKUP(G$5, config!$B$4:$O$14,MATCH($F9,config!$B$6:$O$6,),FALSE)</f>
         <v>UP</v>
       </c>
       <c r="H9" s="8">
-        <f>VLOOKUP(H$5, config!$B$4:$G$14,MATCH($F9,config!$B$6:$G$6,),FALSE)</f>
+        <f>VLOOKUP(H$5, config!$B$4:$O$14,MATCH($F9,config!$B$6:$O$6,),FALSE)</f>
         <v>1</v>
       </c>
       <c r="J9" s="8">
-        <f>VLOOKUP("Value", config!$B$4:$G$14,MATCH($F9,config!$B$6:$G$6,),FALSE)</f>
-        <v>35644</v>
+        <f>VLOOKUP("Value", config!$B$4:$O$14,MATCH($F9,config!$B$6:$O$6,),FALSE)</f>
+        <v>31606</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="C10" s="8" t="str">
-        <f>VLOOKUP(C$5, config!$B$4:$G$14,MATCH($F10,config!$B$6:$G$6,),FALSE)</f>
+        <f>VLOOKUP(C$5, config!$B$4:$O$14,MATCH($F10,config!$B$6:$O$6,),FALSE)</f>
         <v>*CO2*,-*CO2S</v>
       </c>
       <c r="D10" s="8" t="str">
-        <f>VLOOKUP(D$5, config!$B$4:$G$14,MATCH($F10,config!$B$6:$G$6,),FALSE)</f>
+        <f>VLOOKUP(D$5, config!$B$4:$O$14,MATCH($F10,config!$B$6:$O$6,),FALSE)</f>
         <v>ENV</v>
       </c>
       <c r="E10" s="8" t="str">
-        <f>VLOOKUP(E$5, config!$B$4:$G$14,MATCH($F10,config!$B$6:$G$6,),FALSE)</f>
+        <f>VLOOKUP(E$5, config!$B$4:$O$14,MATCH($F10,config!$B$6:$O$6,),FALSE)</f>
         <v>T-A*INT*,T-NAV*</v>
       </c>
       <c r="F10" s="8">
@@ -2753,109 +3369,485 @@
         <v>2021</v>
       </c>
       <c r="I10" s="8">
-        <f>VLOOKUP(I$5, config!$B$4:$G$14,MATCH($F10,config!$B$6:$G$6,),FALSE)</f>
+        <f>VLOOKUP(I$5, config!$B$4:$O$14,MATCH($F10,config!$B$6:$O$6,),FALSE)</f>
         <v>-1</v>
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="C11" s="8" t="str">
-        <f>VLOOKUP(C$5, config!$B$4:$G$14,MATCH($F11,config!$B$6:$G$6,),FALSE)</f>
+        <f>VLOOKUP(C$5, config!$B$4:$O$14,MATCH($F11,config!$B$6:$O$6,),FALSE)</f>
         <v>*CO2*,-*CO2S</v>
       </c>
       <c r="D11" s="8" t="str">
-        <f>VLOOKUP(D$5, config!$B$4:$G$14,MATCH($F11,config!$B$6:$G$6,),FALSE)</f>
+        <f>VLOOKUP(D$5, config!$B$4:$O$14,MATCH($F11,config!$B$6:$O$6,),FALSE)</f>
         <v>ENV</v>
       </c>
       <c r="F11" s="8">
-        <v>2030</v>
+        <v>2022</v>
       </c>
       <c r="G11" s="8" t="str">
-        <f>VLOOKUP(G$5, config!$B$4:$G$14,MATCH($F11,config!$B$6:$G$6,),FALSE)</f>
+        <f>VLOOKUP(G$5, config!$B$4:$O$14,MATCH($F11,config!$B$6:$O$6,),FALSE)</f>
         <v>UP</v>
       </c>
       <c r="H11" s="8">
-        <f>VLOOKUP(H$5, config!$B$4:$G$14,MATCH($F11,config!$B$6:$G$6,),FALSE)</f>
+        <f>VLOOKUP(H$5, config!$B$4:$O$14,MATCH($F11,config!$B$6:$O$6,),FALSE)</f>
         <v>1</v>
       </c>
       <c r="J11" s="8">
-        <f>VLOOKUP("Value", config!$B$4:$G$14,MATCH($F11,config!$B$6:$G$6,),FALSE)</f>
-        <v>12482</v>
+        <f>VLOOKUP("Value", config!$B$4:$O$14,MATCH($F11,config!$B$6:$O$6,),FALSE)</f>
+        <v>100000</v>
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="C12" s="8" t="str">
-        <f>VLOOKUP(C$5, config!$B$4:$G$14,MATCH($F12,config!$B$6:$G$6,),FALSE)</f>
+        <f>VLOOKUP(C$5, config!$B$4:$O$14,MATCH($F12,config!$B$6:$O$6,),FALSE)</f>
         <v>*CO2*,-*CO2S</v>
       </c>
       <c r="D12" s="8" t="str">
-        <f>VLOOKUP(D$5, config!$B$4:$G$14,MATCH($F12,config!$B$6:$G$6,),FALSE)</f>
+        <f>VLOOKUP(D$5, config!$B$4:$O$14,MATCH($F12,config!$B$6:$O$6,),FALSE)</f>
         <v>ENV</v>
       </c>
       <c r="E12" s="8" t="str">
-        <f>VLOOKUP(E$5, config!$B$4:$G$14,MATCH($F12,config!$B$6:$G$6,),FALSE)</f>
+        <f>VLOOKUP(E$5, config!$B$4:$O$14,MATCH($F12,config!$B$6:$O$6,),FALSE)</f>
         <v>T-A*INT*,T-NAV*</v>
       </c>
       <c r="F12" s="8">
         <f>F11</f>
-        <v>2030</v>
+        <v>2022</v>
       </c>
       <c r="I12" s="8">
-        <f>VLOOKUP(I$5, config!$B$4:$G$14,MATCH($F12,config!$B$6:$G$6,),FALSE)</f>
+        <f>VLOOKUP(I$5, config!$B$4:$O$14,MATCH($F12,config!$B$6:$O$6,),FALSE)</f>
         <v>-1</v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="C13" s="8" t="str">
-        <f>VLOOKUP(C$5, config!$B$4:$G$14,MATCH($F13,config!$B$6:$G$6,),FALSE)</f>
+        <f>VLOOKUP(C$5, config!$B$4:$O$14,MATCH($F13,config!$B$6:$O$6,),FALSE)</f>
         <v>*CO2*,-*CO2S</v>
       </c>
       <c r="D13" s="8" t="str">
-        <f>VLOOKUP(D$5, config!$B$4:$G$14,MATCH($F13,config!$B$6:$G$6,),FALSE)</f>
+        <f>VLOOKUP(D$5, config!$B$4:$O$14,MATCH($F13,config!$B$6:$O$6,),FALSE)</f>
         <v>ENV</v>
       </c>
       <c r="F13" s="8">
-        <v>2050</v>
+        <v>2023</v>
       </c>
       <c r="G13" s="8" t="str">
-        <f>VLOOKUP(G$5, config!$B$4:$G$14,MATCH($F13,config!$B$6:$G$6,),FALSE)</f>
+        <f>VLOOKUP(G$5, config!$B$4:$O$14,MATCH($F13,config!$B$6:$O$6,),FALSE)</f>
         <v>UP</v>
       </c>
       <c r="H13" s="8">
-        <f>VLOOKUP(H$5, config!$B$4:$G$14,MATCH($F13,config!$B$6:$G$6,),FALSE)</f>
+        <f>VLOOKUP(H$5, config!$B$4:$O$14,MATCH($F13,config!$B$6:$O$6,),FALSE)</f>
         <v>1</v>
       </c>
       <c r="J13" s="8">
-        <f>VLOOKUP("Value", config!$B$4:$G$14,MATCH($F13,config!$B$6:$G$6,),FALSE)</f>
-        <v>0</v>
+        <f>VLOOKUP("Value", config!$B$4:$O$14,MATCH($F13,config!$B$6:$O$6,),FALSE)</f>
+        <v>100000</v>
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="C14" s="8" t="str">
-        <f>VLOOKUP(C$5, config!$B$4:$G$14,MATCH($F14,config!$B$6:$G$6,),FALSE)</f>
+        <f>VLOOKUP(C$5, config!$B$4:$O$14,MATCH($F14,config!$B$6:$O$6,),FALSE)</f>
         <v>*CO2*,-*CO2S</v>
       </c>
       <c r="D14" s="8" t="str">
-        <f>VLOOKUP(D$5, config!$B$4:$G$14,MATCH($F14,config!$B$6:$G$6,),FALSE)</f>
+        <f>VLOOKUP(D$5, config!$B$4:$O$14,MATCH($F14,config!$B$6:$O$6,),FALSE)</f>
         <v>ENV</v>
       </c>
       <c r="E14" s="8" t="str">
-        <f>VLOOKUP(E$5, config!$B$4:$G$14,MATCH($F14,config!$B$6:$G$6,),FALSE)</f>
+        <f>VLOOKUP(E$5, config!$B$4:$O$14,MATCH($F14,config!$B$6:$O$6,),FALSE)</f>
         <v>T-A*INT*,T-NAV*</v>
       </c>
       <c r="F14" s="8">
+        <f>F13</f>
+        <v>2023</v>
+      </c>
+      <c r="I14" s="8">
+        <f>VLOOKUP(I$5, config!$B$4:$O$14,MATCH($F14,config!$B$6:$O$6,),FALSE)</f>
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="C15" s="8" t="str">
+        <f>VLOOKUP(C$5, config!$B$4:$O$14,MATCH($F15,config!$B$6:$O$6,),FALSE)</f>
+        <v>*CO2*,-*CO2S</v>
+      </c>
+      <c r="D15" s="8" t="str">
+        <f>VLOOKUP(D$5, config!$B$4:$O$14,MATCH($F15,config!$B$6:$O$6,),FALSE)</f>
+        <v>ENV</v>
+      </c>
+      <c r="F15" s="8">
+        <v>2024</v>
+      </c>
+      <c r="G15" s="8" t="str">
+        <f>VLOOKUP(G$5, config!$B$4:$O$14,MATCH($F15,config!$B$6:$O$6,),FALSE)</f>
+        <v>UP</v>
+      </c>
+      <c r="H15" s="8">
+        <f>VLOOKUP(H$5, config!$B$4:$O$14,MATCH($F15,config!$B$6:$O$6,),FALSE)</f>
+        <v>1</v>
+      </c>
+      <c r="J15" s="8">
+        <f>VLOOKUP("Value", config!$B$4:$O$14,MATCH($F15,config!$B$6:$O$6,),FALSE)</f>
+        <v>100000</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="C16" s="8" t="str">
+        <f>VLOOKUP(C$5, config!$B$4:$O$14,MATCH($F16,config!$B$6:$O$6,),FALSE)</f>
+        <v>*CO2*,-*CO2S</v>
+      </c>
+      <c r="D16" s="8" t="str">
+        <f>VLOOKUP(D$5, config!$B$4:$O$14,MATCH($F16,config!$B$6:$O$6,),FALSE)</f>
+        <v>ENV</v>
+      </c>
+      <c r="E16" s="8" t="str">
+        <f>VLOOKUP(E$5, config!$B$4:$O$14,MATCH($F16,config!$B$6:$O$6,),FALSE)</f>
+        <v>T-A*INT*,T-NAV*</v>
+      </c>
+      <c r="F16" s="8">
+        <f>F15</f>
+        <v>2024</v>
+      </c>
+      <c r="I16" s="8">
+        <f>VLOOKUP(I$5, config!$B$4:$O$14,MATCH($F16,config!$B$6:$O$6,),FALSE)</f>
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="17" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C17" s="8" t="str">
+        <f>VLOOKUP(C$5, config!$B$4:$O$14,MATCH($F17,config!$B$6:$O$6,),FALSE)</f>
+        <v>*CO2*,-*CO2S</v>
+      </c>
+      <c r="D17" s="8" t="str">
+        <f>VLOOKUP(D$5, config!$B$4:$O$14,MATCH($F17,config!$B$6:$O$6,),FALSE)</f>
+        <v>ENV</v>
+      </c>
+      <c r="F17" s="8">
+        <v>2025</v>
+      </c>
+      <c r="G17" s="8" t="str">
+        <f>VLOOKUP(G$5, config!$B$4:$O$14,MATCH($F17,config!$B$6:$O$6,),FALSE)</f>
+        <v>UP</v>
+      </c>
+      <c r="H17" s="8">
+        <f>VLOOKUP(H$5, config!$B$4:$O$14,MATCH($F17,config!$B$6:$O$6,),FALSE)</f>
+        <v>1</v>
+      </c>
+      <c r="J17" s="8">
+        <f>VLOOKUP("Value", config!$B$4:$O$14,MATCH($F17,config!$B$6:$O$6,),FALSE)</f>
+        <v>100000</v>
+      </c>
+    </row>
+    <row r="18" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C18" s="8" t="str">
+        <f>VLOOKUP(C$5, config!$B$4:$O$14,MATCH($F18,config!$B$6:$O$6,),FALSE)</f>
+        <v>*CO2*,-*CO2S</v>
+      </c>
+      <c r="D18" s="8" t="str">
+        <f>VLOOKUP(D$5, config!$B$4:$O$14,MATCH($F18,config!$B$6:$O$6,),FALSE)</f>
+        <v>ENV</v>
+      </c>
+      <c r="E18" s="8" t="str">
+        <f>VLOOKUP(E$5, config!$B$4:$O$14,MATCH($F18,config!$B$6:$O$6,),FALSE)</f>
+        <v>T-A*INT*,T-NAV*</v>
+      </c>
+      <c r="F18" s="8">
+        <f>F17</f>
+        <v>2025</v>
+      </c>
+      <c r="I18" s="8">
+        <f>VLOOKUP(I$5, config!$B$4:$O$14,MATCH($F18,config!$B$6:$O$6,),FALSE)</f>
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="19" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C19" s="8" t="str">
+        <f>VLOOKUP(C$5, config!$B$4:$O$14,MATCH($F19,config!$B$6:$O$6,),FALSE)</f>
+        <v>*CO2*,-*CO2S</v>
+      </c>
+      <c r="D19" s="8" t="str">
+        <f>VLOOKUP(D$5, config!$B$4:$O$14,MATCH($F19,config!$B$6:$O$6,),FALSE)</f>
+        <v>ENV</v>
+      </c>
+      <c r="F19" s="8">
+        <v>2026</v>
+      </c>
+      <c r="G19" s="8" t="str">
+        <f>VLOOKUP(G$5, config!$B$4:$O$14,MATCH($F19,config!$B$6:$O$6,),FALSE)</f>
+        <v>UP</v>
+      </c>
+      <c r="H19" s="8">
+        <f>VLOOKUP(H$5, config!$B$4:$O$14,MATCH($F19,config!$B$6:$O$6,),FALSE)</f>
+        <v>1</v>
+      </c>
+      <c r="J19" s="8">
+        <f>VLOOKUP("Value", config!$B$4:$O$14,MATCH($F19,config!$B$6:$O$6,),FALSE)</f>
+        <v>100000</v>
+      </c>
+    </row>
+    <row r="20" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C20" s="8" t="str">
+        <f>VLOOKUP(C$5, config!$B$4:$O$14,MATCH($F20,config!$B$6:$O$6,),FALSE)</f>
+        <v>*CO2*,-*CO2S</v>
+      </c>
+      <c r="D20" s="8" t="str">
+        <f>VLOOKUP(D$5, config!$B$4:$O$14,MATCH($F20,config!$B$6:$O$6,),FALSE)</f>
+        <v>ENV</v>
+      </c>
+      <c r="E20" s="8" t="str">
+        <f>VLOOKUP(E$5, config!$B$4:$O$14,MATCH($F20,config!$B$6:$O$6,),FALSE)</f>
+        <v>T-A*INT*,T-NAV*</v>
+      </c>
+      <c r="F20" s="8">
+        <f>F19</f>
+        <v>2026</v>
+      </c>
+      <c r="I20" s="8">
+        <f>VLOOKUP(I$5, config!$B$4:$O$14,MATCH($F20,config!$B$6:$O$6,),FALSE)</f>
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="21" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C21" s="8" t="str">
+        <f>VLOOKUP(C$5, config!$B$4:$O$14,MATCH($F21,config!$B$6:$O$6,),FALSE)</f>
+        <v>*CO2*,-*CO2S</v>
+      </c>
+      <c r="D21" s="8" t="str">
+        <f>VLOOKUP(D$5, config!$B$4:$O$14,MATCH($F21,config!$B$6:$O$6,),FALSE)</f>
+        <v>ENV</v>
+      </c>
+      <c r="F21" s="8">
+        <v>2027</v>
+      </c>
+      <c r="G21" s="8" t="str">
+        <f>VLOOKUP(G$5, config!$B$4:$O$14,MATCH($F21,config!$B$6:$O$6,),FALSE)</f>
+        <v>UP</v>
+      </c>
+      <c r="H21" s="8">
+        <f>VLOOKUP(H$5, config!$B$4:$O$14,MATCH($F21,config!$B$6:$O$6,),FALSE)</f>
+        <v>1</v>
+      </c>
+      <c r="J21" s="8">
+        <f>VLOOKUP("Value", config!$B$4:$O$14,MATCH($F21,config!$B$6:$O$6,),FALSE)</f>
+        <v>100000</v>
+      </c>
+    </row>
+    <row r="22" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C22" s="8" t="str">
+        <f>VLOOKUP(C$5, config!$B$4:$O$14,MATCH($F22,config!$B$6:$O$6,),FALSE)</f>
+        <v>*CO2*,-*CO2S</v>
+      </c>
+      <c r="D22" s="8" t="str">
+        <f>VLOOKUP(D$5, config!$B$4:$O$14,MATCH($F22,config!$B$6:$O$6,),FALSE)</f>
+        <v>ENV</v>
+      </c>
+      <c r="E22" s="8" t="str">
+        <f>VLOOKUP(E$5, config!$B$4:$O$14,MATCH($F22,config!$B$6:$O$6,),FALSE)</f>
+        <v>T-A*INT*,T-NAV*</v>
+      </c>
+      <c r="F22" s="8">
+        <f>F21</f>
+        <v>2027</v>
+      </c>
+      <c r="I22" s="8">
+        <f>VLOOKUP(I$5, config!$B$4:$O$14,MATCH($F22,config!$B$6:$O$6,),FALSE)</f>
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="23" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C23" s="8" t="str">
+        <f>VLOOKUP(C$5, config!$B$4:$O$14,MATCH($F23,config!$B$6:$O$6,),FALSE)</f>
+        <v>*CO2*,-*CO2S</v>
+      </c>
+      <c r="D23" s="8" t="str">
+        <f>VLOOKUP(D$5, config!$B$4:$O$14,MATCH($F23,config!$B$6:$O$6,),FALSE)</f>
+        <v>ENV</v>
+      </c>
+      <c r="F23" s="8">
+        <v>2028</v>
+      </c>
+      <c r="G23" s="8" t="str">
+        <f>VLOOKUP(G$5, config!$B$4:$O$14,MATCH($F23,config!$B$6:$O$6,),FALSE)</f>
+        <v>UP</v>
+      </c>
+      <c r="H23" s="8">
+        <f>VLOOKUP(H$5, config!$B$4:$O$14,MATCH($F23,config!$B$6:$O$6,),FALSE)</f>
+        <v>1</v>
+      </c>
+      <c r="J23" s="8">
+        <f>VLOOKUP("Value", config!$B$4:$O$14,MATCH($F23,config!$B$6:$O$6,),FALSE)</f>
+        <v>100000</v>
+      </c>
+    </row>
+    <row r="24" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C24" s="8" t="str">
+        <f>VLOOKUP(C$5, config!$B$4:$O$14,MATCH($F24,config!$B$6:$O$6,),FALSE)</f>
+        <v>*CO2*,-*CO2S</v>
+      </c>
+      <c r="D24" s="8" t="str">
+        <f>VLOOKUP(D$5, config!$B$4:$O$14,MATCH($F24,config!$B$6:$O$6,),FALSE)</f>
+        <v>ENV</v>
+      </c>
+      <c r="E24" s="8" t="str">
+        <f>VLOOKUP(E$5, config!$B$4:$O$14,MATCH($F24,config!$B$6:$O$6,),FALSE)</f>
+        <v>T-A*INT*,T-NAV*</v>
+      </c>
+      <c r="F24" s="8">
+        <f>F23</f>
+        <v>2028</v>
+      </c>
+      <c r="I24" s="8">
+        <f>VLOOKUP(I$5, config!$B$4:$O$14,MATCH($F24,config!$B$6:$O$6,),FALSE)</f>
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="25" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C25" s="8" t="str">
+        <f>VLOOKUP(C$5, config!$B$4:$O$14,MATCH($F25,config!$B$6:$O$6,),FALSE)</f>
+        <v>*CO2*,-*CO2S</v>
+      </c>
+      <c r="D25" s="8" t="str">
+        <f>VLOOKUP(D$5, config!$B$4:$O$14,MATCH($F25,config!$B$6:$O$6,),FALSE)</f>
+        <v>ENV</v>
+      </c>
+      <c r="F25" s="8">
+        <v>2029</v>
+      </c>
+      <c r="G25" s="8" t="str">
+        <f>VLOOKUP(G$5, config!$B$4:$O$14,MATCH($F25,config!$B$6:$O$6,),FALSE)</f>
+        <v>UP</v>
+      </c>
+      <c r="H25" s="8">
+        <f>VLOOKUP(H$5, config!$B$4:$O$14,MATCH($F25,config!$B$6:$O$6,),FALSE)</f>
+        <v>1</v>
+      </c>
+      <c r="J25" s="8">
+        <f>VLOOKUP("Value", config!$B$4:$O$14,MATCH($F25,config!$B$6:$O$6,),FALSE)</f>
+        <v>100000</v>
+      </c>
+    </row>
+    <row r="26" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C26" s="8" t="str">
+        <f>VLOOKUP(C$5, config!$B$4:$O$14,MATCH($F26,config!$B$6:$O$6,),FALSE)</f>
+        <v>*CO2*,-*CO2S</v>
+      </c>
+      <c r="D26" s="8" t="str">
+        <f>VLOOKUP(D$5, config!$B$4:$O$14,MATCH($F26,config!$B$6:$O$6,),FALSE)</f>
+        <v>ENV</v>
+      </c>
+      <c r="E26" s="8" t="str">
+        <f>VLOOKUP(E$5, config!$B$4:$O$14,MATCH($F26,config!$B$6:$O$6,),FALSE)</f>
+        <v>T-A*INT*,T-NAV*</v>
+      </c>
+      <c r="F26" s="8">
+        <f>F25</f>
+        <v>2029</v>
+      </c>
+      <c r="I26" s="8">
+        <f>VLOOKUP(I$5, config!$B$4:$O$14,MATCH($F26,config!$B$6:$O$6,),FALSE)</f>
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="27" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C27" s="8" t="str">
+        <f>VLOOKUP(C$5, config!$B$4:$O$14,MATCH($F27,config!$B$6:$O$6,),FALSE)</f>
+        <v>*CO2*,-*CO2S</v>
+      </c>
+      <c r="D27" s="8" t="str">
+        <f>VLOOKUP(D$5, config!$B$4:$O$14,MATCH($F27,config!$B$6:$O$6,),FALSE)</f>
+        <v>ENV</v>
+      </c>
+      <c r="F27" s="8">
+        <v>2030</v>
+      </c>
+      <c r="G27" s="8" t="str">
+        <f>VLOOKUP(G$5, config!$B$4:$O$14,MATCH($F27,config!$B$6:$O$6,),FALSE)</f>
+        <v>UP</v>
+      </c>
+      <c r="H27" s="8">
+        <f>VLOOKUP(H$5, config!$B$4:$O$14,MATCH($F27,config!$B$6:$O$6,),FALSE)</f>
+        <v>1</v>
+      </c>
+      <c r="J27" s="8">
+        <f>VLOOKUP("Value", config!$B$4:$O$14,MATCH($F27,config!$B$6:$O$6,),FALSE)</f>
+        <v>12482</v>
+      </c>
+    </row>
+    <row r="28" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C28" s="8" t="str">
+        <f>VLOOKUP(C$5, config!$B$4:$O$14,MATCH($F28,config!$B$6:$O$6,),FALSE)</f>
+        <v>*CO2*,-*CO2S</v>
+      </c>
+      <c r="D28" s="8" t="str">
+        <f>VLOOKUP(D$5, config!$B$4:$O$14,MATCH($F28,config!$B$6:$O$6,),FALSE)</f>
+        <v>ENV</v>
+      </c>
+      <c r="E28" s="8" t="str">
+        <f>VLOOKUP(E$5, config!$B$4:$O$14,MATCH($F28,config!$B$6:$O$6,),FALSE)</f>
+        <v>T-A*INT*,T-NAV*</v>
+      </c>
+      <c r="F28" s="8">
+        <f>F27</f>
+        <v>2030</v>
+      </c>
+      <c r="I28" s="8">
+        <f>VLOOKUP(I$5, config!$B$4:$O$14,MATCH($F28,config!$B$6:$O$6,),FALSE)</f>
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="29" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C29" s="8" t="str">
+        <f>VLOOKUP(C$5, config!$B$4:$O$14,MATCH($F29,config!$B$6:$O$6,),FALSE)</f>
+        <v>*CO2*,-*CO2S</v>
+      </c>
+      <c r="D29" s="8" t="str">
+        <f>VLOOKUP(D$5, config!$B$4:$O$14,MATCH($F29,config!$B$6:$O$6,),FALSE)</f>
+        <v>ENV</v>
+      </c>
+      <c r="F29" s="8">
         <v>2050</v>
       </c>
-      <c r="I14" s="8">
-        <f>VLOOKUP(I$5, config!$B$4:$G$14,MATCH($F14,config!$B$6:$G$6,),FALSE)</f>
+      <c r="G29" s="8" t="str">
+        <f>VLOOKUP(G$5, config!$B$4:$O$14,MATCH($F29,config!$B$6:$O$6,),FALSE)</f>
+        <v>UP</v>
+      </c>
+      <c r="H29" s="8">
+        <f>VLOOKUP(H$5, config!$B$4:$O$14,MATCH($F29,config!$B$6:$O$6,),FALSE)</f>
+        <v>1</v>
+      </c>
+      <c r="J29" s="8">
+        <f>VLOOKUP("Value", config!$B$4:$O$14,MATCH($F29,config!$B$6:$O$6,),FALSE)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C30" s="8" t="str">
+        <f>VLOOKUP(C$5, config!$B$4:$O$14,MATCH($F30,config!$B$6:$O$6,),FALSE)</f>
+        <v>*CO2*,-*CO2S</v>
+      </c>
+      <c r="D30" s="8" t="str">
+        <f>VLOOKUP(D$5, config!$B$4:$O$14,MATCH($F30,config!$B$6:$O$6,),FALSE)</f>
+        <v>ENV</v>
+      </c>
+      <c r="E30" s="8" t="str">
+        <f>VLOOKUP(E$5, config!$B$4:$O$14,MATCH($F30,config!$B$6:$O$6,),FALSE)</f>
+        <v>T-A*INT*,T-NAV*</v>
+      </c>
+      <c r="F30" s="8">
+        <v>2050</v>
+      </c>
+      <c r="I30" s="8">
+        <f>VLOOKUP(I$5, config!$B$4:$O$14,MATCH($F30,config!$B$6:$O$6,),FALSE)</f>
         <v>-1</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="F15" s="8">
+    <row r="31" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="F31" s="8">
         <v>0</v>
       </c>
-      <c r="J15" s="8">
-        <f>VLOOKUP("Value", config!$B$4:$G$14,MATCH($F15,config!$B$6:$G$6,),FALSE)</f>
+      <c r="J31" s="8">
+        <f>VLOOKUP("Value", config!$B$4:$O$14,MATCH($F31,config!$B$6:$O$6,),FALSE)</f>
         <v>5</v>
       </c>
     </row>
@@ -2870,7 +3862,7 @@
   <dimension ref="B2:H4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="M27" sqref="M27"/>
+      <selection activeCell="I4" sqref="I4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>